<commit_message>
repair error in conditionSheet.xslx
</commit_message>
<xml_diff>
--- a/Working Documents/Non-Mapping Documents/conditions/conditionSheet.xlsx
+++ b/Working Documents/Non-Mapping Documents/conditions/conditionSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/tgis_uw_edu/Documents/Documents/gitRepos/MARC2RDA/Working Documents/Non-Mapping Documents/conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7F3775B-5C79-40D3-9290-1E3D22EAB6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E874AACF-E2BE-4BB0-BA20-5A5C2F88D57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{963FDEDD-EF49-4E2C-BBB2-9FE1880800B6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5100" windowWidth="29040" windowHeight="15840" xr2:uid="{7D32C1ED-353D-44C4-961E-1F28F2CA6F1A}"/>
+    <workbookView xWindow="-28920" yWindow="5100" windowWidth="29040" windowHeight="15840" xr2:uid="{FAE3BA0F-A317-4367-9EF5-DEF39CE65FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,14 +680,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837154DB-E67C-4B15-AACF-62CF6155D652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C214185-C1CB-410A-B3D5-0941C65BD571}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.9453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.47265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">

</xml_diff>